<commit_message>
fixed CA prog stats on illspouse, updated CA takeups
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B38685-8A9D-4B60-ACC6-6FCCDC061C87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13E3132-2ECE-45F0-A7DE-E0A17CBC694A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27600" yWindow="7350" windowWidth="21600" windowHeight="14130" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_obsolote_Combined" sheetId="4" r:id="rId1"/>
@@ -560,7 +560,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +600,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,7 +651,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -707,6 +713,8 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1038,7 +1046,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L12" sqref="L12"/>
+      <selection pane="topRight" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2124,13 +2132,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2173,104 +2181,222 @@
       </c>
       <c r="B2" s="2">
         <f>AVERAGE(E2:I2)</f>
-        <v>17282000</v>
+        <v>13260469</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <v>13260469</v>
+      </c>
       <c r="F2" s="2">
-        <v>17282000</v>
-      </c>
-      <c r="G2" s="2"/>
+        <v>13260469</v>
+      </c>
+      <c r="G2" s="2">
+        <v>13260469</v>
+      </c>
+      <c r="H2" s="2">
+        <v>13260469</v>
+      </c>
+      <c r="I2" s="2">
+        <v>13260469</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B21" si="0">AVERAGE(E3:I3)</f>
-        <v>17282000</v>
+        <f t="shared" ref="B3:B20" si="0">AVERAGE(E3:I3)</f>
+        <v>13260469</v>
+      </c>
+      <c r="E3" s="2">
+        <v>13260469</v>
       </c>
       <c r="F3" s="2">
-        <v>17282000</v>
+        <v>13260469</v>
+      </c>
+      <c r="G3" s="2">
+        <v>13260469</v>
+      </c>
+      <c r="H3" s="2">
+        <v>13260469</v>
+      </c>
+      <c r="I3" s="2">
+        <v>13260469</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" si="0"/>
-        <v>2.6971878254831615E-2</v>
-      </c>
-      <c r="F4">
+      <c r="B4" s="54">
+        <f>AVERAGE(E4:I4)</f>
+        <v>3.5215149630077186E-2</v>
+      </c>
+      <c r="E4" s="54">
+        <f>E10/E$3</f>
+        <v>3.5307800953344862E-2</v>
+      </c>
+      <c r="F4" s="54">
         <f>F10/F$3</f>
-        <v>2.6971878254831615E-2</v>
+        <v>3.5151697877352603E-2</v>
+      </c>
+      <c r="G4" s="54">
+        <f t="shared" ref="G4:I4" si="1">G10/G$3</f>
+        <v>3.5602586906994013E-2</v>
+      </c>
+      <c r="H4" s="54">
+        <f t="shared" si="1"/>
+        <v>3.5026287531760757E-2</v>
+      </c>
+      <c r="I4" s="54">
+        <f t="shared" si="1"/>
+        <v>3.4987374880933696E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="54">
         <f t="shared" si="0"/>
-        <v>9.7343478764031939E-3</v>
-      </c>
-      <c r="F5">
+        <v>1.2874567257010291E-2</v>
+      </c>
+      <c r="E5" s="54">
+        <f>E11/E$3</f>
+        <v>1.2472258711211496E-2</v>
+      </c>
+      <c r="F5" s="54">
         <f>F11/F$3</f>
-        <v>9.7343478764031939E-3</v>
+        <v>1.2686504527102321E-2</v>
+      </c>
+      <c r="G5" s="54">
+        <f t="shared" ref="G5:I5" si="2">G11/G$3</f>
+        <v>1.3045843250340543E-2</v>
+      </c>
+      <c r="H5" s="54">
+        <f t="shared" si="2"/>
+        <v>1.327004346528015E-2</v>
+      </c>
+      <c r="I5" s="54">
+        <f t="shared" si="2"/>
+        <v>1.2898186331116945E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="54">
         <f t="shared" si="0"/>
-        <v>1.2065096632334221E-2</v>
-      </c>
-      <c r="F6">
+        <v>1.6424200380846257E-2</v>
+      </c>
+      <c r="E6" s="54">
+        <f>E12/E$3</f>
+        <v>1.5121938748923586E-2</v>
+      </c>
+      <c r="F6" s="54">
         <f>F12/F$3</f>
-        <v>1.2065096632334221E-2</v>
+        <v>1.5724104479260877E-2</v>
+      </c>
+      <c r="G6" s="54">
+        <f t="shared" ref="G6:I6" si="3">G12/G$3</f>
+        <v>1.6352739861614247E-2</v>
+      </c>
+      <c r="H6" s="54">
+        <f t="shared" si="3"/>
+        <v>1.7138911150125988E-2</v>
+      </c>
+      <c r="I6" s="54">
+        <f t="shared" si="3"/>
+        <v>1.7783307664306594E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="54">
         <f>AVERAGE(E7:I7)</f>
-        <v>3.5533405855803728E-4</v>
-      </c>
-      <c r="F7">
+        <v>4.8269131959058153E-4</v>
+      </c>
+      <c r="E7" s="54">
+        <f>E13/E$3</f>
+        <v>4.4066948159978352E-4</v>
+      </c>
+      <c r="F7" s="54">
         <f>F13/F$3</f>
-        <v>3.5533405855803728E-4</v>
+        <v>4.6309698397545366E-4</v>
+      </c>
+      <c r="G7" s="54">
+        <f t="shared" ref="G7:I7" si="4">G13/G$3</f>
+        <v>4.6301744681881158E-4</v>
+      </c>
+      <c r="H7" s="54">
+        <f t="shared" si="4"/>
+        <v>5.1241687605468552E-4</v>
+      </c>
+      <c r="I7" s="54">
+        <f t="shared" si="4"/>
+        <v>5.3425580950417363E-4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="54">
         <f t="shared" si="0"/>
-        <v>1.2244811657909964E-4</v>
-      </c>
-      <c r="F8">
+        <v>8.1277200678196227E-4</v>
+      </c>
+      <c r="E8" s="54">
+        <f>E14/E$3</f>
+        <v>7.2278031795104691E-4</v>
+      </c>
+      <c r="F8" s="54">
         <f>F14/F$3</f>
-        <v>1.2244811657909964E-4</v>
+        <v>7.467628482823647E-4</v>
+      </c>
+      <c r="G8" s="54">
+        <f t="shared" ref="G8:I8" si="5">G14/G$3</f>
+        <v>8.5372372575962419E-4</v>
+      </c>
+      <c r="H8" s="54">
+        <f t="shared" si="5"/>
+        <v>8.4248608401407221E-4</v>
+      </c>
+      <c r="I8" s="54">
+        <f t="shared" si="5"/>
+        <v>8.9810705790270313E-4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="54">
         <f t="shared" si="0"/>
-        <v>5.470514986691355E-4</v>
-      </c>
-      <c r="F9">
+        <v>7.7357802352239575E-4</v>
+      </c>
+      <c r="E9" s="54">
+        <f>E15/E$3</f>
+        <v>6.8983306699031536E-4</v>
+      </c>
+      <c r="F9" s="54">
         <f>F15/F$3</f>
-        <v>5.470514986691355E-4</v>
+        <v>7.1295698515640735E-4</v>
+      </c>
+      <c r="G9" s="54">
+        <f t="shared" ref="G9:I9" si="6">G15/G$3</f>
+        <v>7.4344919474567605E-4</v>
+      </c>
+      <c r="H9" s="54">
+        <f t="shared" si="6"/>
+        <v>8.3077796871287141E-4</v>
+      </c>
+      <c r="I9" s="54">
+        <f t="shared" si="6"/>
+        <v>8.9087290200670882E-4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
@@ -2282,19 +2408,19 @@
         <v>466969.4</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:F10" si="1">C16-C11</f>
+        <f t="shared" ref="C10:F10" si="7">C16-C11</f>
         <v>488011</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>461036</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>468198</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>466128</v>
       </c>
       <c r="G10" s="2">
@@ -2377,26 +2503,29 @@
       <c r="A13" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>6400.7132799999999</v>
+      </c>
+      <c r="C13" s="25">
         <v>5616.66</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="25">
         <v>5537.6639999999998</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="25">
         <v>5843.4839999999995</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="25">
         <v>6140.8832000000002</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="25">
         <v>6139.8284999999996</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="25">
         <v>6794.8881000000001</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="25">
         <v>7084.4825999999994</v>
       </c>
     </row>
@@ -2404,53 +2533,59 @@
       <c r="A14" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
-        <v>1977.0643200000002</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1982.4837119999997</v>
-      </c>
-      <c r="E14" s="2">
-        <v>2051.0628839999999</v>
-      </c>
-      <c r="F14" s="2">
-        <v>2116.1483507200001</v>
-      </c>
-      <c r="G14" s="2">
-        <v>4112.457129299999</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2298.0311554200002</v>
-      </c>
-      <c r="I14" s="2">
-        <v>2374.7185675199999</v>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>10777.738000000001</v>
+      </c>
+      <c r="C14" s="25">
+        <v>9414.5920000000006</v>
+      </c>
+      <c r="D14" s="25">
+        <v>9485.5679999999993</v>
+      </c>
+      <c r="E14" s="25">
+        <v>9584.4060000000009</v>
+      </c>
+      <c r="F14" s="25">
+        <v>9902.4256000000005</v>
+      </c>
+      <c r="G14" s="25">
+        <v>11320.776999999998</v>
+      </c>
+      <c r="H14" s="25">
+        <v>11171.7606</v>
+      </c>
+      <c r="I14" s="25">
+        <v>11909.3208</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2">
-        <v>9414.5919999999987</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>10258.0074</v>
+      </c>
+      <c r="C15" s="25">
+        <v>9414.5920000000006</v>
+      </c>
+      <c r="D15" s="25">
         <v>9247.1039999999994</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="25">
         <v>9147.51</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="25">
         <v>9454.1440000000002</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="25">
         <v>9858.4850000000006</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="25">
         <v>11016.505500000001</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="25">
         <v>11813.3925</v>
       </c>
     </row>
@@ -2644,11 +2779,11 @@
         <v>5590876250</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" ref="H21:I21" si="2">SUM(H19:H20)</f>
+        <f t="shared" ref="H21:I21" si="8">SUM(H19:H20)</f>
         <v>5941076368</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6356405026</v>
       </c>
       <c r="K21" t="s">
@@ -2679,128 +2814,128 @@
         <v>34</v>
       </c>
     </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.45">
+      <c r="E33">
+        <v>2011</v>
+      </c>
+      <c r="F33">
+        <v>2012</v>
+      </c>
+      <c r="G33">
+        <v>2013</v>
+      </c>
+      <c r="H33">
+        <v>2014</v>
+      </c>
+      <c r="I33">
+        <v>2015</v>
+      </c>
+      <c r="J33">
+        <v>2016</v>
+      </c>
+      <c r="K33">
+        <v>2017</v>
+      </c>
+      <c r="L33">
+        <v>2018</v>
+      </c>
+      <c r="M33">
+        <v>2019</v>
+      </c>
+    </row>
     <row r="34" spans="4:13" x14ac:dyDescent="0.45">
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
       <c r="E34">
-        <v>2011</v>
+        <v>5208</v>
       </c>
       <c r="F34">
-        <v>2012</v>
+        <v>5616.66</v>
       </c>
       <c r="G34">
-        <v>2013</v>
+        <v>5537.6639999999998</v>
       </c>
       <c r="H34">
-        <v>2014</v>
+        <v>5843.4839999999995</v>
       </c>
       <c r="I34">
-        <v>2015</v>
+        <v>6140.8832000000002</v>
       </c>
       <c r="J34">
-        <v>2016</v>
+        <v>6139.8284999999996</v>
       </c>
       <c r="K34">
-        <v>2017</v>
+        <v>6794.8881000000001</v>
       </c>
       <c r="L34">
-        <v>2018</v>
+        <v>7084.4825999999994</v>
       </c>
       <c r="M34">
-        <v>2019</v>
+        <v>8985.2909999999993</v>
       </c>
     </row>
     <row r="35" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D35" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E35">
-        <v>5208</v>
+        <v>9140.0400000000009</v>
       </c>
       <c r="F35">
-        <v>5616.66</v>
+        <v>9414.5920000000006</v>
       </c>
       <c r="G35">
-        <v>5537.6639999999998</v>
+        <v>9485.5679999999993</v>
       </c>
       <c r="H35">
-        <v>5843.4839999999995</v>
+        <v>9584.4060000000009</v>
       </c>
       <c r="I35">
-        <v>6140.8832000000002</v>
+        <v>9902.4256000000005</v>
       </c>
       <c r="J35">
-        <v>6139.8284999999996</v>
+        <v>11320.776999999998</v>
       </c>
       <c r="K35">
-        <v>6794.8881000000001</v>
+        <v>11171.7606</v>
       </c>
       <c r="L35">
-        <v>7084.4825999999994</v>
+        <v>11909.3208</v>
       </c>
       <c r="M35">
-        <v>8985.2909999999993</v>
+        <v>14505.236999999999</v>
       </c>
     </row>
     <row r="36" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D36" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E36">
-        <v>1828.0080000000003</v>
+        <v>9322.32</v>
       </c>
       <c r="F36">
-        <v>1977.0643200000002</v>
+        <v>9414.5919999999987</v>
       </c>
       <c r="G36">
-        <v>1982.4837119999997</v>
+        <v>9247.1039999999994</v>
       </c>
       <c r="H36">
-        <v>2051.0628839999999</v>
+        <v>9147.51</v>
       </c>
       <c r="I36">
-        <v>2116.1483507200001</v>
+        <v>9454.1440000000002</v>
       </c>
       <c r="J36">
-        <v>4112.457129299999</v>
+        <v>9858.4850000000006</v>
       </c>
       <c r="K36">
-        <v>2298.0311554200002</v>
+        <v>11016.505500000001</v>
       </c>
       <c r="L36">
-        <v>2374.7185675199999</v>
+        <v>11813.3925</v>
       </c>
       <c r="M36">
-        <v>3178.0974266999992</v>
-      </c>
-    </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.45">
-      <c r="D37" t="s">
-        <v>138</v>
-      </c>
-      <c r="E37">
-        <v>9322.32</v>
-      </c>
-      <c r="F37">
-        <v>9414.5919999999987</v>
-      </c>
-      <c r="G37">
-        <v>9247.1039999999994</v>
-      </c>
-      <c r="H37">
-        <v>9147.51</v>
-      </c>
-      <c r="I37">
-        <v>9454.1440000000002</v>
-      </c>
-      <c r="J37">
-        <v>9858.4850000000006</v>
-      </c>
-      <c r="K37">
-        <v>11016.505500000001</v>
-      </c>
-      <c r="L37">
-        <v>11813.3925</v>
-      </c>
-      <c r="M37">
         <v>15116.286</v>
       </c>
     </row>
@@ -2953,7 +3088,7 @@
         <v>120</v>
       </c>
       <c r="B5" s="54">
-        <f t="shared" ref="B4:B15" si="1">AVERAGE(E5:I5)</f>
+        <f t="shared" ref="B5:B9" si="1">AVERAGE(E5:I5)</f>
         <v>8.3666509937933373E-3</v>
       </c>
       <c r="E5" s="50">
@@ -2986,23 +3121,23 @@
         <v>9.1691430830897896E-3</v>
       </c>
       <c r="E6" s="50">
-        <f>E12/E$3</f>
+        <f t="shared" ref="E6:F9" si="3">E12/E$3</f>
         <v>8.6047147690709678E-3</v>
       </c>
       <c r="F6" s="50">
-        <f>F12/F$3</f>
+        <f t="shared" si="3"/>
         <v>8.631348410022853E-3</v>
       </c>
       <c r="G6" s="50">
-        <f t="shared" ref="G6:I6" si="3">G12/G$3</f>
+        <f t="shared" ref="G6:I6" si="4">G12/G$3</f>
         <v>8.6422750319518332E-3</v>
       </c>
       <c r="H6" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.8022042411000099E-3</v>
       </c>
       <c r="I6" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0165172963303281E-2</v>
       </c>
     </row>
@@ -3015,23 +3150,23 @@
         <v>4.1493846775297779E-4</v>
       </c>
       <c r="E7" s="50">
-        <f>E13/E$3</f>
+        <f t="shared" si="3"/>
         <v>4.0735812378974855E-4</v>
       </c>
       <c r="F7" s="50">
-        <f>F13/F$3</f>
+        <f t="shared" si="3"/>
         <v>3.6433454994439375E-4</v>
       </c>
       <c r="G7" s="50">
-        <f t="shared" ref="G7:I7" si="4">G13/G$3</f>
+        <f t="shared" ref="G7:I7" si="5">G13/G$3</f>
         <v>3.8345613832010701E-4</v>
       </c>
       <c r="H7" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5379626698790934E-4</v>
       </c>
       <c r="I7" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.6574725972273016E-4</v>
       </c>
     </row>
@@ -3044,23 +3179,23 @@
         <v>5.2099499185113019E-4</v>
       </c>
       <c r="E8" s="50">
-        <f>E14/E$3</f>
+        <f t="shared" si="3"/>
         <v>5.4018487161389963E-4</v>
       </c>
       <c r="F8" s="50">
-        <f>F14/F$3</f>
+        <f t="shared" si="3"/>
         <v>4.9340527148045827E-4</v>
       </c>
       <c r="G8" s="50">
-        <f t="shared" ref="G8:I8" si="5">G14/G$3</f>
+        <f t="shared" ref="G8:I8" si="6">G14/G$3</f>
         <v>4.5789375021127647E-4</v>
       </c>
       <c r="H8" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.7228182353027545E-4</v>
       </c>
       <c r="I8" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.4120924241974136E-4</v>
       </c>
     </row>
@@ -3073,23 +3208,23 @@
         <v>7.3495190749795045E-4</v>
       </c>
       <c r="E9" s="50">
-        <f>E15/E$3</f>
+        <f t="shared" si="3"/>
         <v>7.1705956408924724E-4</v>
       </c>
       <c r="F9" s="50">
-        <f>F15/F$3</f>
+        <f t="shared" si="3"/>
         <v>6.392073828452719E-4</v>
       </c>
       <c r="G9" s="50">
-        <f t="shared" ref="G9:I9" si="6">G15/G$3</f>
+        <f t="shared" ref="G9:I9" si="7">G15/G$3</f>
         <v>6.6823122234412231E-4</v>
       </c>
       <c r="H9" s="50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.9832631468602867E-4</v>
       </c>
       <c r="I9" s="50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.5193505352508189E-4</v>
       </c>
     </row>
@@ -3132,7 +3267,7 @@
         <v>104</v>
       </c>
       <c r="B11" s="38">
-        <f t="shared" ref="B11:B15" si="7">AVERAGE(E11:I11)</f>
+        <f t="shared" ref="B11:B14" si="8">AVERAGE(E11:I11)</f>
         <v>24502.799999999999</v>
       </c>
       <c r="C11" t="s">
@@ -3169,7 +3304,7 @@
         <v>105</v>
       </c>
       <c r="B12" s="38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26853</v>
       </c>
       <c r="D12" t="s">
@@ -3205,7 +3340,7 @@
         <v>106</v>
       </c>
       <c r="B13" s="38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1215.2</v>
       </c>
       <c r="C13" s="15"/>
@@ -3242,7 +3377,7 @@
         <v>107</v>
       </c>
       <c r="B14" s="38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1525.8</v>
       </c>
       <c r="C14" s="15"/>
@@ -3279,7 +3414,7 @@
         <v>108</v>
       </c>
       <c r="B15" s="38">
-        <f>AVERAGE(E15:I15)</f>
+        <f t="shared" ref="B15:B20" si="9">AVERAGE(E15:I15)</f>
         <v>2152.4</v>
       </c>
       <c r="C15" s="15"/>
@@ -3316,7 +3451,7 @@
         <v>109</v>
       </c>
       <c r="B16" s="2">
-        <f>AVERAGE(E16:I16)</f>
+        <f t="shared" si="9"/>
         <v>91046</v>
       </c>
       <c r="C16" s="2">
@@ -3348,7 +3483,7 @@
         <v>110</v>
       </c>
       <c r="B17" s="2">
-        <f>AVERAGE(E17:I17)</f>
+        <f t="shared" si="9"/>
         <v>32124</v>
       </c>
       <c r="C17" s="2">
@@ -3380,7 +3515,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="3">
-        <f>AVERAGE(E18:I18)</f>
+        <f t="shared" si="9"/>
         <v>412060000</v>
       </c>
       <c r="C18" s="4">
@@ -3419,7 +3554,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="3">
-        <f>AVERAGE(E19:I19)</f>
+        <f t="shared" si="9"/>
         <v>90180000</v>
       </c>
       <c r="C19" s="4">
@@ -3458,35 +3593,35 @@
         <v>9</v>
       </c>
       <c r="B20" s="3">
-        <f>AVERAGE(E20:I20)</f>
+        <f t="shared" si="9"/>
         <v>502240000</v>
       </c>
       <c r="C20" s="3">
-        <f>SUM(C18:C19)</f>
+        <f t="shared" ref="C20:I20" si="10">SUM(C18:C19)</f>
         <v>506700000</v>
       </c>
       <c r="D20" s="3">
-        <f>SUM(D18:D19)</f>
+        <f t="shared" si="10"/>
         <v>513100000</v>
       </c>
       <c r="E20" s="3">
-        <f>SUM(E18:E19)</f>
+        <f t="shared" si="10"/>
         <v>506600000</v>
       </c>
       <c r="F20" s="3">
-        <f>SUM(F18:F19)</f>
+        <f t="shared" si="10"/>
         <v>505400000</v>
       </c>
       <c r="G20" s="3">
-        <f>SUM(G18:G19)</f>
+        <f t="shared" si="10"/>
         <v>502900000</v>
       </c>
       <c r="H20" s="3">
-        <f>SUM(H18:H19)</f>
+        <f t="shared" si="10"/>
         <v>501900000</v>
       </c>
       <c r="I20" s="3">
-        <f>SUM(I18:I19)</f>
+        <f t="shared" si="10"/>
         <v>494400000</v>
       </c>
       <c r="J20" t="s">
@@ -3761,7 +3896,7 @@
         <v>2.8504038123626806E-2</v>
       </c>
       <c r="F5" s="50">
-        <f t="shared" ref="E5:G5" si="2">F11/F$2</f>
+        <f t="shared" ref="F5:G5" si="2">F11/F$2</f>
         <v>2.2868951407774864E-2</v>
       </c>
       <c r="G5" s="50">
@@ -4771,7 +4906,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D82DAC-6301-4138-9431-4FB81094A8CB}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:J14"/>
@@ -5056,7 +5191,8 @@
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="G9" s="56">
-        <v>0.32840000000000003</v>
+        <f>1-SUM(G6:G8,G10)</f>
+        <v>3.6399999999999988E-2</v>
       </c>
       <c r="H9" s="56">
         <v>8.9999999999999993E-3</v>
@@ -5101,155 +5237,194 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B11">
+      <c r="A11" s="57"/>
+      <c r="B11" s="57">
         <v>2011</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="57">
         <v>2012</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="57">
         <v>2013</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="57">
         <v>2014</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="57">
         <v>2015</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="57">
         <v>2016</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="57">
         <v>2017</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="57">
         <v>2018</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="57">
         <v>2019</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="A12" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="58">
         <f>B$2*B$7</f>
         <v>5208</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="58">
         <f t="shared" ref="C12:J12" si="0">C$2*C$7</f>
         <v>5616.66</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="58">
         <f t="shared" si="0"/>
         <v>5537.6639999999998</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="58">
         <f t="shared" si="0"/>
         <v>5843.4839999999995</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="58">
         <f t="shared" si="0"/>
         <v>6140.8832000000002</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="58">
         <f t="shared" si="0"/>
         <v>6139.8284999999996</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="58">
         <f t="shared" si="0"/>
         <v>6794.8881000000001</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="58">
         <f t="shared" si="0"/>
         <v>7084.4825999999994</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="58">
         <f t="shared" si="0"/>
         <v>8985.2909999999993</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="A13" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="25">
-        <f>B$12*(B$6+B$9)</f>
-        <v>1828.0080000000003</v>
-      </c>
-      <c r="C13" s="25">
-        <f t="shared" ref="C13:J13" si="1">C$12*(C$6+C$9)</f>
-        <v>1977.0643200000002</v>
-      </c>
-      <c r="D13" s="25">
+      <c r="B13" s="58">
+        <f>B$2*(B$6+B$9)</f>
+        <v>9140.0400000000009</v>
+      </c>
+      <c r="C13" s="58">
+        <f t="shared" ref="C13:J13" si="1">C$2*(C$6+C$9)</f>
+        <v>9414.5920000000006</v>
+      </c>
+      <c r="D13" s="58">
         <f t="shared" si="1"/>
-        <v>1982.4837119999997</v>
-      </c>
-      <c r="E13" s="25">
+        <v>9485.5679999999993</v>
+      </c>
+      <c r="E13" s="58">
         <f t="shared" si="1"/>
-        <v>2051.0628839999999</v>
-      </c>
-      <c r="F13" s="25">
+        <v>9584.4060000000009</v>
+      </c>
+      <c r="F13" s="58">
         <f t="shared" si="1"/>
-        <v>2116.1483507200001</v>
-      </c>
-      <c r="G13" s="25">
+        <v>9902.4256000000005</v>
+      </c>
+      <c r="G13" s="58">
+        <f>G$2*(G$6+G$9)</f>
+        <v>11320.776999999998</v>
+      </c>
+      <c r="H13" s="58">
         <f t="shared" si="1"/>
-        <v>4112.457129299999</v>
-      </c>
-      <c r="H13" s="25">
+        <v>11171.7606</v>
+      </c>
+      <c r="I13" s="58">
         <f t="shared" si="1"/>
-        <v>2298.0311554200002</v>
-      </c>
-      <c r="I13" s="25">
+        <v>11909.3208</v>
+      </c>
+      <c r="J13" s="58">
         <f t="shared" si="1"/>
-        <v>2374.7185675199999</v>
-      </c>
-      <c r="J13" s="25">
-        <f t="shared" si="1"/>
-        <v>3178.0974266999992</v>
+        <v>14505.236999999999</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="A14" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="58">
         <f>B$2*B$8</f>
         <v>9322.32</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="58">
         <f t="shared" ref="C14:J14" si="2">C$2*C$8</f>
         <v>9414.5919999999987</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="58">
         <f t="shared" si="2"/>
         <v>9247.1039999999994</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="58">
         <f t="shared" si="2"/>
         <v>9147.51</v>
       </c>
-      <c r="F14" s="25">
-        <f t="shared" si="2"/>
+      <c r="F14" s="58">
+        <f>F$2*F$8</f>
         <v>9454.1440000000002</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="58">
         <f t="shared" si="2"/>
         <v>9858.4850000000006</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="58">
         <f t="shared" si="2"/>
         <v>11016.505500000001</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="58">
         <f t="shared" si="2"/>
         <v>11813.3925</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="58">
         <f t="shared" si="2"/>
         <v>15116.286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B15" s="27">
+        <f>SUM(B6:B10)</f>
+        <v>1.0010000000000001</v>
+      </c>
+      <c r="C15" s="27">
+        <f>SUM(C6:C10)</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="27">
+        <f>SUM(D6:D10)</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="E15" s="27">
+        <f>SUM(E6:E10)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="F15" s="27">
+        <f>SUM(F6:F10)</f>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G15" s="27">
+        <f>SUM(G6:G10)</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="27">
+        <f>SUM(H6:H10)</f>
+        <v>1.0001</v>
+      </c>
+      <c r="I15" s="27">
+        <f>SUM(I6:I10)</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="27">
+        <f>SUM(J6:J10)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model testing done for IB2, TBD - NJ/NB large CI
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13E3132-2ECE-45F0-A7DE-E0A17CBC694A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0BE93D-E4F5-4E2F-84A3-59FC39C32682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_obsolote_Combined" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="140">
   <si>
     <t>Participated for own illness leave</t>
   </si>
@@ -297,9 +297,6 @@
     <t>dervied</t>
   </si>
   <si>
-    <t>avg</t>
-  </si>
-  <si>
     <t>CPI</t>
   </si>
   <si>
@@ -454,6 +451,12 @@
   </si>
   <si>
     <t>illparent</t>
+  </si>
+  <si>
+    <t>weekly benefit cap</t>
+  </si>
+  <si>
+    <t>wage replcement ratio</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -715,6 +718,9 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="6" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="40" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1590,7 +1596,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="6"/>
@@ -2138,7 +2144,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2151,7 +2157,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="52">
         <v>2012</v>
@@ -2227,200 +2233,200 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="54">
         <f>AVERAGE(E4:I4)</f>
         <v>3.5215149630077186E-2</v>
       </c>
       <c r="E4" s="54">
-        <f>E10/E$3</f>
+        <f t="shared" ref="E4:F9" si="1">E10/E$3</f>
         <v>3.5307800953344862E-2</v>
       </c>
       <c r="F4" s="54">
-        <f>F10/F$3</f>
+        <f t="shared" si="1"/>
         <v>3.5151697877352603E-2</v>
       </c>
       <c r="G4" s="54">
-        <f t="shared" ref="G4:I4" si="1">G10/G$3</f>
+        <f t="shared" ref="G4:I4" si="2">G10/G$3</f>
         <v>3.5602586906994013E-2</v>
       </c>
       <c r="H4" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.5026287531760757E-2</v>
       </c>
       <c r="I4" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4987374880933696E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="54">
         <f t="shared" si="0"/>
         <v>1.2874567257010291E-2</v>
       </c>
       <c r="E5" s="54">
-        <f>E11/E$3</f>
+        <f t="shared" si="1"/>
         <v>1.2472258711211496E-2</v>
       </c>
       <c r="F5" s="54">
-        <f>F11/F$3</f>
+        <f t="shared" si="1"/>
         <v>1.2686504527102321E-2</v>
       </c>
       <c r="G5" s="54">
-        <f t="shared" ref="G5:I5" si="2">G11/G$3</f>
+        <f t="shared" ref="G5:I5" si="3">G11/G$3</f>
         <v>1.3045843250340543E-2</v>
       </c>
       <c r="H5" s="54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.327004346528015E-2</v>
       </c>
       <c r="I5" s="54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2898186331116945E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="54">
         <f t="shared" si="0"/>
         <v>1.6424200380846257E-2</v>
       </c>
       <c r="E6" s="54">
-        <f>E12/E$3</f>
+        <f t="shared" si="1"/>
         <v>1.5121938748923586E-2</v>
       </c>
       <c r="F6" s="54">
-        <f>F12/F$3</f>
+        <f t="shared" si="1"/>
         <v>1.5724104479260877E-2</v>
       </c>
       <c r="G6" s="54">
-        <f t="shared" ref="G6:I6" si="3">G12/G$3</f>
+        <f t="shared" ref="G6:I6" si="4">G12/G$3</f>
         <v>1.6352739861614247E-2</v>
       </c>
       <c r="H6" s="54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7138911150125988E-2</v>
       </c>
       <c r="I6" s="54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7783307664306594E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="54">
         <f>AVERAGE(E7:I7)</f>
         <v>4.8269131959058153E-4</v>
       </c>
       <c r="E7" s="54">
-        <f>E13/E$3</f>
+        <f t="shared" si="1"/>
         <v>4.4066948159978352E-4</v>
       </c>
       <c r="F7" s="54">
-        <f>F13/F$3</f>
+        <f t="shared" si="1"/>
         <v>4.6309698397545366E-4</v>
       </c>
       <c r="G7" s="54">
-        <f t="shared" ref="G7:I7" si="4">G13/G$3</f>
+        <f t="shared" ref="G7:I7" si="5">G13/G$3</f>
         <v>4.6301744681881158E-4</v>
       </c>
       <c r="H7" s="54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.1241687605468552E-4</v>
       </c>
       <c r="I7" s="54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.3425580950417363E-4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="54">
         <f t="shared" si="0"/>
         <v>8.1277200678196227E-4</v>
       </c>
       <c r="E8" s="54">
-        <f>E14/E$3</f>
+        <f t="shared" si="1"/>
         <v>7.2278031795104691E-4</v>
       </c>
       <c r="F8" s="54">
-        <f>F14/F$3</f>
+        <f t="shared" si="1"/>
         <v>7.467628482823647E-4</v>
       </c>
       <c r="G8" s="54">
-        <f t="shared" ref="G8:I8" si="5">G14/G$3</f>
+        <f t="shared" ref="G8:I8" si="6">G14/G$3</f>
         <v>8.5372372575962419E-4</v>
       </c>
       <c r="H8" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.4248608401407221E-4</v>
       </c>
       <c r="I8" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.9810705790270313E-4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="54">
         <f t="shared" si="0"/>
         <v>7.7357802352239575E-4</v>
       </c>
       <c r="E9" s="54">
-        <f>E15/E$3</f>
+        <f t="shared" si="1"/>
         <v>6.8983306699031536E-4</v>
       </c>
       <c r="F9" s="54">
-        <f>F15/F$3</f>
+        <f t="shared" si="1"/>
         <v>7.1295698515640735E-4</v>
       </c>
       <c r="G9" s="54">
-        <f t="shared" ref="G9:I9" si="6">G15/G$3</f>
+        <f t="shared" ref="G9:I9" si="7">G15/G$3</f>
         <v>7.4344919474567605E-4</v>
       </c>
       <c r="H9" s="54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.3077796871287141E-4</v>
       </c>
       <c r="I9" s="54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.9087290200670882E-4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>466969.4</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:F10" si="7">C16-C11</f>
+        <f t="shared" ref="C10:F10" si="8">C16-C11</f>
         <v>488011</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>461036</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>468198</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>466128</v>
       </c>
       <c r="G10" s="2">
@@ -2438,7 +2444,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
@@ -2468,7 +2474,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
@@ -2501,7 +2507,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
@@ -2531,7 +2537,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
@@ -2561,7 +2567,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
@@ -2591,7 +2597,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
@@ -2618,16 +2624,10 @@
       <c r="I16" s="2">
         <v>634985</v>
       </c>
-      <c r="K16">
-        <v>2012</v>
-      </c>
-      <c r="L16" s="4">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
@@ -2654,14 +2654,8 @@
       <c r="I17" s="2">
         <v>35529</v>
       </c>
-      <c r="K17">
-        <v>2013</v>
-      </c>
-      <c r="L17" s="4">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -2671,14 +2665,8 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="K18">
-        <v>2014</v>
-      </c>
-      <c r="L18" s="4">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2707,14 +2695,8 @@
       <c r="I19" s="2">
         <v>5492544463</v>
       </c>
-      <c r="K19">
-        <v>2015</v>
-      </c>
-      <c r="L19" s="4">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2743,14 +2725,8 @@
       <c r="I20" s="2">
         <v>863860563</v>
       </c>
-      <c r="K20">
-        <v>2016</v>
-      </c>
-      <c r="L20" s="4">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -2779,39 +2755,122 @@
         <v>5590876250</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" ref="H21:I21" si="8">SUM(H19:H20)</f>
+        <f t="shared" ref="H21:I21" si="9">SUM(H19:H20)</f>
         <v>5941076368</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6356405026</v>
       </c>
-      <c r="K21" t="s">
-        <v>86</v>
-      </c>
-      <c r="L21" s="4">
-        <f>AVERAGE(L16:L20)</f>
-        <v>1082.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F24">
+        <v>2012</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1011</v>
+      </c>
+      <c r="H24">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F25">
+        <v>2013</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1067</v>
+      </c>
+      <c r="H25">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>34</v>
+      </c>
+      <c r="F26" s="15">
+        <v>2014</v>
+      </c>
+      <c r="G26" s="53">
+        <v>1075</v>
+      </c>
+      <c r="H26">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F27" s="15">
+        <v>2015</v>
+      </c>
+      <c r="G27" s="53">
+        <v>1129</v>
+      </c>
+      <c r="H27">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F28" s="15">
+        <v>2016</v>
+      </c>
+      <c r="G28" s="53">
+        <v>1129</v>
+      </c>
+      <c r="H28">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F29" s="15">
+        <v>2017</v>
+      </c>
+      <c r="G29" s="53">
+        <v>1173</v>
+      </c>
+      <c r="H29">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F30" s="15">
+        <v>2018</v>
+      </c>
+      <c r="G30" s="53">
+        <v>1215</v>
+      </c>
+      <c r="H30">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F31" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="60">
+        <f>AVERAGE(G26:G30)</f>
+        <v>1144.2</v>
+      </c>
+      <c r="H31" s="61">
+        <f>AVERAGE(H26:H30)</f>
+        <v>0.57000000000000006</v>
       </c>
     </row>
     <row r="33" spans="4:13" x14ac:dyDescent="0.45">
@@ -2845,7 +2904,7 @@
     </row>
     <row r="34" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E34">
         <v>5208</v>
@@ -2877,7 +2936,7 @@
     </row>
     <row r="35" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35">
         <v>9140.0400000000009</v>
@@ -2909,7 +2968,7 @@
     </row>
     <row r="36" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E36">
         <v>9322.32</v>
@@ -2971,7 +3030,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="52">
         <v>2012</v>
@@ -3006,7 +3065,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2">
         <f>AVERAGE(E2:I2)</f>
@@ -3032,7 +3091,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2">
         <f>AVERAGE(E3:I3)</f>
@@ -3056,7 +3115,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="54">
         <f>AVERAGE(E4:I4)</f>
@@ -3085,7 +3144,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="54">
         <f t="shared" ref="B5:B9" si="1">AVERAGE(E5:I5)</f>
@@ -3114,7 +3173,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="54">
         <f t="shared" si="1"/>
@@ -3143,7 +3202,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="54">
         <f t="shared" si="1"/>
@@ -3172,7 +3231,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="54">
         <f t="shared" si="1"/>
@@ -3201,7 +3260,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="54">
         <f t="shared" si="1"/>
@@ -3230,7 +3289,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="38">
         <f>AVERAGE(E10:I10)</f>
@@ -3264,7 +3323,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="38">
         <f t="shared" ref="B11:B14" si="8">AVERAGE(E11:I11)</f>
@@ -3301,7 +3360,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="38">
         <f t="shared" si="8"/>
@@ -3337,7 +3396,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="38">
         <f t="shared" si="8"/>
@@ -3374,7 +3433,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="38">
         <f t="shared" si="8"/>
@@ -3411,7 +3470,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="38">
         <f t="shared" ref="B15:B20" si="9">AVERAGE(E15:I15)</f>
@@ -3448,7 +3507,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="9"/>
@@ -3480,7 +3539,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="9"/>
@@ -3654,7 +3713,7 @@
         <v>74</v>
       </c>
       <c r="G29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.45">
@@ -3665,7 +3724,7 @@
         <v>572</v>
       </c>
       <c r="G30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.45">
@@ -3676,7 +3735,7 @@
         <v>584</v>
       </c>
       <c r="G31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.45">
@@ -3687,7 +3746,7 @@
         <v>595</v>
       </c>
       <c r="G32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="5:19" x14ac:dyDescent="0.45">
@@ -3698,7 +3757,7 @@
         <v>604</v>
       </c>
       <c r="G33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="5:19" x14ac:dyDescent="0.45">
@@ -3709,7 +3768,7 @@
         <v>615</v>
       </c>
       <c r="G34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="5:19" x14ac:dyDescent="0.45">
@@ -3720,7 +3779,7 @@
         <v>633</v>
       </c>
       <c r="G35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
@@ -3736,12 +3795,12 @@
         <v>637</v>
       </c>
       <c r="G36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="5:19" x14ac:dyDescent="0.45">
       <c r="E39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F39" s="4">
         <f>AVERAGE(F32:F36)</f>
@@ -3800,7 +3859,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="5">
         <f t="shared" ref="B2:B15" si="0">AVERAGE(C2:E2)</f>
@@ -3824,7 +3883,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5">
         <f t="shared" si="0"/>
@@ -4022,7 +4081,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="5">
         <f t="shared" si="0"/>
@@ -4051,7 +4110,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="5">
         <f>AVERAGE(C11:E11)</f>
@@ -4080,7 +4139,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="5">
         <f>AVERAGE(C12:E12)</f>
@@ -4104,7 +4163,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="5">
         <f t="shared" si="0"/>
@@ -4128,7 +4187,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="5">
         <f>AVERAGE(C14:E14)</f>
@@ -4152,7 +4211,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" si="0"/>
@@ -4176,7 +4235,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" ref="B16:B22" si="8">AVERAGE(C16:E16)</f>
@@ -4200,7 +4259,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="5">
         <f t="shared" si="8"/>
@@ -4229,7 +4288,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5">
@@ -4250,7 +4309,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5">
@@ -4358,7 +4417,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C26" s="39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
@@ -4722,7 +4781,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
@@ -4868,7 +4927,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
@@ -4981,7 +5040,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="27">
         <v>0.66900000000000004</v>
@@ -5013,7 +5072,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="27">
         <v>0.32900000000000001</v>
@@ -5045,7 +5104,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="27">
         <v>2E-3</v>
@@ -5173,7 +5232,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="27">
         <v>1.2999999999999999E-2</v>
@@ -5206,7 +5265,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="27">
         <v>9.1999999999999998E-2</v>
@@ -5268,7 +5327,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="58">
         <f>B$2*B$7</f>
@@ -5309,7 +5368,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" s="58">
         <f>B$2*(B$6+B$9)</f>
@@ -5350,7 +5409,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14" s="58">
         <f>B$2*B$8</f>
@@ -5391,39 +5450,39 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B15" s="27">
-        <f>SUM(B6:B10)</f>
+        <f t="shared" ref="B15:J15" si="3">SUM(B6:B10)</f>
         <v>1.0010000000000001</v>
       </c>
       <c r="C15" s="27">
-        <f>SUM(C6:C10)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D15" s="27">
-        <f>SUM(D6:D10)</f>
+        <f t="shared" si="3"/>
         <v>1.0009999999999999</v>
       </c>
       <c r="E15" s="27">
-        <f>SUM(E6:E10)</f>
+        <f t="shared" si="3"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="F15" s="27">
-        <f>SUM(F6:F10)</f>
+        <f t="shared" si="3"/>
         <v>0.99990000000000001</v>
       </c>
       <c r="G15" s="27">
-        <f>SUM(G6:G10)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H15" s="27">
-        <f>SUM(H6:H10)</f>
+        <f t="shared" si="3"/>
         <v>1.0001</v>
       </c>
       <c r="I15" s="27">
-        <f>SUM(I6:I10)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J15" s="27">
-        <f>SUM(J6:J10)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
plot validation results vs state prog stats
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0BE93D-E4F5-4E2F-84A3-59FC39C32682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFF7478-2555-4B1B-89A2-FD7EFE53CCC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_obsolote_Combined" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed 18 take up with 1.02x on denom, commit docs
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFF7478-2555-4B1B-89A2-FD7EFE53CCC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AFA479-481D-4D4D-B3B9-3F8466BC4D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_obsolote_Combined" sheetId="4" r:id="rId1"/>
@@ -654,7 +654,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -721,6 +721,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="6" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="40" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1051,8 +1052,8 @@
   <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A14" sqref="A14:XFD14"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2140,11 +2141,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2187,24 +2188,29 @@
       </c>
       <c r="B2" s="2">
         <f>AVERAGE(E2:I2)</f>
-        <v>13260469</v>
+        <v>13525678.380000001</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>13260469</v>
+        <f>13260469*1.02</f>
+        <v>13525678.380000001</v>
       </c>
       <c r="F2" s="2">
-        <v>13260469</v>
+        <f t="shared" ref="F2:I3" si="0">13260469*1.02</f>
+        <v>13525678.380000001</v>
       </c>
       <c r="G2" s="2">
-        <v>13260469</v>
+        <f t="shared" si="0"/>
+        <v>13525678.380000001</v>
       </c>
       <c r="H2" s="2">
-        <v>13260469</v>
+        <f t="shared" si="0"/>
+        <v>13525678.380000001</v>
       </c>
       <c r="I2" s="2">
-        <v>13260469</v>
+        <f t="shared" si="0"/>
+        <v>13525678.380000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -2212,197 +2218,202 @@
         <v>27</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B20" si="0">AVERAGE(E3:I3)</f>
-        <v>13260469</v>
+        <f>AVERAGE(E3:I3)</f>
+        <v>13525678.380000001</v>
       </c>
       <c r="E3" s="2">
-        <v>13260469</v>
+        <f t="shared" ref="E3:I3" si="1">13260469*1.02</f>
+        <v>13525678.380000001</v>
       </c>
       <c r="F3" s="2">
-        <v>13260469</v>
+        <f t="shared" si="0"/>
+        <v>13525678.380000001</v>
       </c>
       <c r="G3" s="2">
-        <v>13260469</v>
+        <f t="shared" si="0"/>
+        <v>13525678.380000001</v>
       </c>
       <c r="H3" s="2">
-        <v>13260469</v>
+        <f t="shared" si="0"/>
+        <v>13525678.380000001</v>
       </c>
       <c r="I3" s="2">
-        <v>13260469</v>
+        <f t="shared" si="0"/>
+        <v>13525678.380000001</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="62">
         <f>AVERAGE(E4:I4)</f>
-        <v>3.5215149630077186E-2</v>
+        <v>3.4524656500075669E-2</v>
       </c>
       <c r="E4" s="54">
-        <f t="shared" ref="E4:F9" si="1">E10/E$3</f>
-        <v>3.5307800953344862E-2</v>
+        <f>E10/E$3</f>
+        <v>3.4615491130730258E-2</v>
       </c>
       <c r="F4" s="54">
-        <f t="shared" si="1"/>
-        <v>3.5151697877352603E-2</v>
+        <f t="shared" ref="E4:F9" si="2">F10/F$3</f>
+        <v>3.4462448899365297E-2</v>
       </c>
       <c r="G4" s="54">
-        <f t="shared" ref="G4:I4" si="2">G10/G$3</f>
-        <v>3.5602586906994013E-2</v>
+        <f t="shared" ref="G4:I4" si="3">G10/G$3</f>
+        <v>3.490449696764119E-2</v>
       </c>
       <c r="H4" s="54">
-        <f t="shared" si="2"/>
-        <v>3.5026287531760757E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.4339497580157599E-2</v>
       </c>
       <c r="I4" s="54">
-        <f t="shared" si="2"/>
-        <v>3.4987374880933696E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.4301347922484016E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="54">
-        <f t="shared" si="0"/>
-        <v>1.2874567257010291E-2</v>
+      <c r="B5" s="62">
+        <f t="shared" ref="B3:B20" si="4">AVERAGE(E5:I5)</f>
+        <v>1.2622124761774794E-2</v>
       </c>
       <c r="E5" s="54">
-        <f t="shared" si="1"/>
-        <v>1.2472258711211496E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.22277046188348E-2</v>
       </c>
       <c r="F5" s="54">
-        <f t="shared" si="1"/>
-        <v>1.2686504527102321E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.2437749536374824E-2</v>
       </c>
       <c r="G5" s="54">
-        <f t="shared" ref="G5:I5" si="3">G11/G$3</f>
-        <v>1.3045843250340543E-2</v>
+        <f t="shared" ref="G5:I5" si="5">G11/G$3</f>
+        <v>1.2790042402294649E-2</v>
       </c>
       <c r="H5" s="54">
-        <f t="shared" si="3"/>
-        <v>1.327004346528015E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.3009846534588381E-2</v>
       </c>
       <c r="I5" s="54">
-        <f t="shared" si="3"/>
-        <v>1.2898186331116945E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.2645280716781318E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="54">
-        <f t="shared" si="0"/>
-        <v>1.6424200380846257E-2</v>
+      <c r="B6" s="62">
+        <f t="shared" si="4"/>
+        <v>1.6102157236123783E-2</v>
       </c>
       <c r="E6" s="54">
-        <f t="shared" si="1"/>
-        <v>1.5121938748923586E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4825430146003515E-2</v>
       </c>
       <c r="F6" s="54">
-        <f t="shared" si="1"/>
-        <v>1.5724104479260877E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.5415788705157722E-2</v>
       </c>
       <c r="G6" s="54">
-        <f t="shared" ref="G6:I6" si="4">G12/G$3</f>
-        <v>1.6352739861614247E-2</v>
+        <f t="shared" ref="G6:I6" si="6">G12/G$3</f>
+        <v>1.6032097903543378E-2</v>
       </c>
       <c r="H6" s="54">
-        <f t="shared" si="4"/>
-        <v>1.7138911150125988E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.6802854068750966E-2</v>
       </c>
       <c r="I6" s="54">
-        <f t="shared" si="4"/>
-        <v>1.7783307664306594E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.7434615357163327E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="54">
+      <c r="B7" s="62">
         <f>AVERAGE(E7:I7)</f>
-        <v>4.8269131959058153E-4</v>
+        <v>4.7322678391233488E-4</v>
       </c>
       <c r="E7" s="54">
-        <f t="shared" si="1"/>
-        <v>4.4066948159978352E-4</v>
+        <f t="shared" si="2"/>
+        <v>4.3202890352919947E-4</v>
       </c>
       <c r="F7" s="54">
-        <f t="shared" si="1"/>
-        <v>4.6309698397545366E-4</v>
+        <f t="shared" si="2"/>
+        <v>4.540166509563271E-4</v>
       </c>
       <c r="G7" s="54">
-        <f t="shared" ref="G7:I7" si="5">G13/G$3</f>
-        <v>4.6301744681881158E-4</v>
+        <f t="shared" ref="G7:I7" si="7">G13/G$3</f>
+        <v>4.5393867335177606E-4</v>
       </c>
       <c r="H7" s="54">
-        <f t="shared" si="5"/>
-        <v>5.1241687605468552E-4</v>
+        <f t="shared" si="7"/>
+        <v>5.0236948632812308E-4</v>
       </c>
       <c r="I7" s="54">
-        <f t="shared" si="5"/>
-        <v>5.3425580950417363E-4</v>
+        <f t="shared" si="7"/>
+        <v>5.2378020539624857E-4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="54">
-        <f t="shared" si="0"/>
-        <v>8.1277200678196227E-4</v>
+      <c r="B8" s="62">
+        <f t="shared" si="4"/>
+        <v>7.9683530076662956E-4</v>
       </c>
       <c r="E8" s="54">
-        <f t="shared" si="1"/>
-        <v>7.2278031795104691E-4</v>
+        <f t="shared" si="2"/>
+        <v>7.0860815485396754E-4</v>
       </c>
       <c r="F8" s="54">
-        <f t="shared" si="1"/>
-        <v>7.467628482823647E-4</v>
+        <f t="shared" si="2"/>
+        <v>7.3212043949251438E-4</v>
       </c>
       <c r="G8" s="54">
-        <f t="shared" ref="G8:I8" si="6">G14/G$3</f>
-        <v>8.5372372575962419E-4</v>
+        <f t="shared" ref="G8:I8" si="8">G14/G$3</f>
+        <v>8.3698404486237665E-4</v>
       </c>
       <c r="H8" s="54">
-        <f t="shared" si="6"/>
-        <v>8.4248608401407221E-4</v>
+        <f t="shared" si="8"/>
+        <v>8.2596674903340401E-4</v>
       </c>
       <c r="I8" s="54">
-        <f t="shared" si="6"/>
-        <v>8.9810705790270313E-4</v>
+        <f t="shared" si="8"/>
+        <v>8.8049711559088533E-4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="54">
-        <f t="shared" si="0"/>
-        <v>7.7357802352239575E-4</v>
+      <c r="B9" s="62">
+        <f t="shared" si="4"/>
+        <v>7.58409826982741E-4</v>
       </c>
       <c r="E9" s="54">
-        <f t="shared" si="1"/>
-        <v>6.8983306699031536E-4</v>
+        <f t="shared" si="2"/>
+        <v>6.7630692842187779E-4</v>
       </c>
       <c r="F9" s="54">
-        <f t="shared" si="1"/>
-        <v>7.1295698515640735E-4</v>
+        <f t="shared" si="2"/>
+        <v>6.9897743642785028E-4</v>
       </c>
       <c r="G9" s="54">
-        <f t="shared" ref="G9:I9" si="7">G15/G$3</f>
-        <v>7.4344919474567605E-4</v>
+        <f t="shared" ref="G9:I9" si="9">G15/G$3</f>
+        <v>7.2887175955458434E-4</v>
       </c>
       <c r="H9" s="54">
-        <f t="shared" si="7"/>
-        <v>8.3077796871287141E-4</v>
+        <f t="shared" si="9"/>
+        <v>8.1448820462046211E-4</v>
       </c>
       <c r="I9" s="54">
-        <f t="shared" si="7"/>
-        <v>8.9087290200670882E-4</v>
+        <f t="shared" si="9"/>
+        <v>8.7340480588893018E-4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
@@ -2410,23 +2421,23 @@
         <v>122</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>466969.4</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:F10" si="8">C16-C11</f>
+        <f t="shared" ref="C10:F10" si="10">C16-C11</f>
         <v>488011</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>461036</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>468198</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>466128</v>
       </c>
       <c r="G10" s="2">
@@ -2447,7 +2458,7 @@
         <v>126</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>170722.8</v>
       </c>
       <c r="C11" s="2">
@@ -2477,7 +2488,7 @@
         <v>127</v>
       </c>
       <c r="B12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>217792.6</v>
       </c>
       <c r="C12" s="2">
@@ -2510,7 +2521,7 @@
         <v>124</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6400.7132799999999</v>
       </c>
       <c r="C13" s="25">
@@ -2540,7 +2551,7 @@
         <v>125</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10777.738000000001</v>
       </c>
       <c r="C14" s="25">
@@ -2570,7 +2581,7 @@
         <v>123</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10258.0074</v>
       </c>
       <c r="C15" s="25">
@@ -2600,7 +2611,7 @@
         <v>128</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>637692.19999999995</v>
       </c>
       <c r="C16" s="2">
@@ -2630,7 +2641,7 @@
         <v>129</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>30913.8</v>
       </c>
       <c r="C17" s="2">
@@ -2671,7 +2682,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4967943707.8000002</v>
       </c>
       <c r="C19" s="3">
@@ -2701,7 +2712,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>713791714.39999998</v>
       </c>
       <c r="C20" s="3">
@@ -2755,11 +2766,11 @@
         <v>5590876250</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" ref="H21:I21" si="9">SUM(H19:H20)</f>
+        <f t="shared" ref="H21:I21" si="11">SUM(H19:H20)</f>
         <v>5941076368</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6356405026</v>
       </c>
     </row>
@@ -3012,10 +3023,10 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3068,25 +3079,30 @@
         <v>89</v>
       </c>
       <c r="B2" s="2">
-        <f>AVERAGE(E2:I2)</f>
-        <v>2928627</v>
+        <f>AVERAGE(E2:I2)*1.02</f>
+        <v>3046943.5308000003</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>2928627</v>
+        <f>2928627*1.02</f>
+        <v>2987199.54</v>
       </c>
       <c r="F2" s="2">
-        <v>2928627</v>
+        <f t="shared" ref="F2:I3" si="0">2928627*1.02</f>
+        <v>2987199.54</v>
       </c>
       <c r="G2" s="2">
-        <v>2928627</v>
+        <f t="shared" si="0"/>
+        <v>2987199.54</v>
       </c>
       <c r="H2" s="2">
-        <v>2928627</v>
+        <f t="shared" si="0"/>
+        <v>2987199.54</v>
       </c>
       <c r="I2" s="2">
-        <v>2928627</v>
+        <f t="shared" si="0"/>
+        <v>2987199.54</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -3094,197 +3110,202 @@
         <v>90</v>
       </c>
       <c r="B3" s="2">
-        <f>AVERAGE(E3:I3)</f>
-        <v>2928627</v>
+        <f>AVERAGE(E3:I3)*1.02</f>
+        <v>3046943.5308000003</v>
       </c>
       <c r="E3" s="2">
-        <v>2928627</v>
+        <f t="shared" ref="E3:I3" si="1">2928627*1.02</f>
+        <v>2987199.54</v>
       </c>
       <c r="F3" s="2">
-        <v>2928627</v>
+        <f t="shared" si="0"/>
+        <v>2987199.54</v>
       </c>
       <c r="G3" s="2">
-        <v>2928627</v>
+        <f t="shared" si="0"/>
+        <v>2987199.54</v>
       </c>
       <c r="H3" s="2">
-        <v>2928627</v>
+        <f t="shared" si="0"/>
+        <v>2987199.54</v>
       </c>
       <c r="I3" s="2">
-        <v>2928627</v>
+        <f t="shared" si="0"/>
+        <v>2987199.54</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="62">
         <f>AVERAGE(E4:I4)</f>
-        <v>2.2659218807994326E-2</v>
+        <v>2.2214920399994436E-2</v>
       </c>
       <c r="E4" s="50">
         <f>E10/E$2</f>
-        <v>2.3829596599362089E-2</v>
+        <v>2.3362349607217735E-2</v>
       </c>
       <c r="F4" s="50">
         <f>F10/F$2</f>
-        <v>2.2886151087181811E-2</v>
+        <v>2.2437403026648831E-2</v>
       </c>
       <c r="G4" s="50">
-        <f t="shared" ref="G4:I4" si="0">G10/G$2</f>
-        <v>2.1924608357431655E-2</v>
+        <f t="shared" ref="G4:I4" si="2">G10/G$2</f>
+        <v>2.1494714075913388E-2</v>
       </c>
       <c r="H4" s="50">
-        <f t="shared" si="0"/>
-        <v>2.2335722507509492E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.1897767164224993E-2</v>
       </c>
       <c r="I4" s="50">
-        <f t="shared" si="0"/>
-        <v>2.2320015488486583E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.1882368125967239E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="54">
-        <f t="shared" ref="B5:B9" si="1">AVERAGE(E5:I5)</f>
-        <v>8.3666509937933373E-3</v>
+      <c r="B5" s="62">
+        <f t="shared" ref="B5:B9" si="3">AVERAGE(E5:I5)</f>
+        <v>8.2025990135228804E-3</v>
       </c>
       <c r="E5" s="50">
         <f>E11/E$2</f>
-        <v>8.2294535971975946E-3</v>
+        <v>8.0680917619584264E-3</v>
       </c>
       <c r="F5" s="50">
         <f>F11/F$2</f>
-        <v>8.2420875038029771E-3</v>
+        <v>8.0804779449048791E-3</v>
       </c>
       <c r="G5" s="50">
-        <f t="shared" ref="G5:I5" si="2">G11/G$2</f>
-        <v>8.152967243694742E-3</v>
+        <f t="shared" ref="G5:I5" si="4">G11/G$2</f>
+        <v>7.9931051408771974E-3</v>
       </c>
       <c r="H5" s="50">
-        <f t="shared" si="2"/>
-        <v>8.6067635106826506E-3</v>
+        <f t="shared" si="4"/>
+        <v>8.4380034418457366E-3</v>
       </c>
       <c r="I5" s="50">
-        <f t="shared" si="2"/>
-        <v>8.6019831135887223E-3</v>
+        <f t="shared" si="4"/>
+        <v>8.433316778028159E-3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="54">
-        <f t="shared" si="1"/>
-        <v>9.1691430830897896E-3</v>
+      <c r="B6" s="62">
+        <f t="shared" si="3"/>
+        <v>8.9893559638135178E-3</v>
       </c>
       <c r="E6" s="50">
-        <f t="shared" ref="E6:F9" si="3">E12/E$3</f>
-        <v>8.6047147690709678E-3</v>
+        <f t="shared" ref="E6:F9" si="5">E12/E$3</f>
+        <v>8.4359948716382031E-3</v>
       </c>
       <c r="F6" s="50">
-        <f t="shared" si="3"/>
-        <v>8.631348410022853E-3</v>
+        <f t="shared" si="5"/>
+        <v>8.4621062843361315E-3</v>
       </c>
       <c r="G6" s="50">
-        <f t="shared" ref="G6:I6" si="4">G12/G$3</f>
-        <v>8.6422750319518332E-3</v>
+        <f t="shared" ref="G6:I6" si="6">G12/G$3</f>
+        <v>8.4728186587763061E-3</v>
       </c>
       <c r="H6" s="50">
-        <f t="shared" si="4"/>
-        <v>9.8022042411000099E-3</v>
+        <f t="shared" si="6"/>
+        <v>9.6100041579411863E-3</v>
       </c>
       <c r="I6" s="50">
-        <f t="shared" si="4"/>
-        <v>1.0165172963303281E-2</v>
+        <f t="shared" si="6"/>
+        <v>9.9658558463757655E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="54">
-        <f t="shared" si="1"/>
-        <v>4.1493846775297779E-4</v>
+      <c r="B7" s="62">
+        <f t="shared" si="3"/>
+        <v>4.0680241936566443E-4</v>
       </c>
       <c r="E7" s="50">
-        <f t="shared" si="3"/>
-        <v>4.0735812378974855E-4</v>
+        <f t="shared" si="5"/>
+        <v>3.9937070959779271E-4</v>
       </c>
       <c r="F7" s="50">
-        <f t="shared" si="3"/>
-        <v>3.6433454994439375E-4</v>
+        <f t="shared" si="5"/>
+        <v>3.5719073523960169E-4</v>
       </c>
       <c r="G7" s="50">
-        <f t="shared" ref="G7:I7" si="5">G13/G$3</f>
-        <v>3.8345613832010701E-4</v>
+        <f t="shared" ref="G7:I7" si="7">G13/G$3</f>
+        <v>3.7593739050990882E-4</v>
       </c>
       <c r="H7" s="50">
-        <f t="shared" si="5"/>
-        <v>4.5379626698790934E-4</v>
+        <f t="shared" si="7"/>
+        <v>4.4489830096853855E-4</v>
       </c>
       <c r="I7" s="50">
-        <f t="shared" si="5"/>
-        <v>4.6574725972273016E-4</v>
+        <f t="shared" si="7"/>
+        <v>4.5661496051248052E-4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="54">
-        <f t="shared" si="1"/>
-        <v>5.2099499185113019E-4</v>
+      <c r="B8" s="62">
+        <f t="shared" si="3"/>
+        <v>5.1077940377561792E-4</v>
       </c>
       <c r="E8" s="50">
-        <f t="shared" si="3"/>
-        <v>5.4018487161389963E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.2959301138617604E-4</v>
       </c>
       <c r="F8" s="50">
-        <f t="shared" si="3"/>
-        <v>4.9340527148045827E-4</v>
+        <f t="shared" si="5"/>
+        <v>4.8373065831417474E-4</v>
       </c>
       <c r="G8" s="50">
-        <f t="shared" ref="G8:I8" si="6">G14/G$3</f>
-        <v>4.5789375021127647E-4</v>
+        <f t="shared" ref="G8:I8" si="8">G14/G$3</f>
+        <v>4.489154413836044E-4</v>
       </c>
       <c r="H8" s="50">
-        <f t="shared" si="6"/>
-        <v>5.7228182353027545E-4</v>
+        <f t="shared" si="8"/>
+        <v>5.6106061130419156E-4</v>
       </c>
       <c r="I8" s="50">
-        <f t="shared" si="6"/>
-        <v>5.4120924241974136E-4</v>
+        <f t="shared" si="8"/>
+        <v>5.3059729648994257E-4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="54">
-        <f t="shared" si="1"/>
-        <v>7.3495190749795045E-4</v>
+      <c r="B9" s="62">
+        <f t="shared" si="3"/>
+        <v>7.2054108578230444E-4</v>
       </c>
       <c r="E9" s="50">
-        <f t="shared" si="3"/>
-        <v>7.1705956408924724E-4</v>
+        <f t="shared" si="5"/>
+        <v>7.0299957263651692E-4</v>
       </c>
       <c r="F9" s="50">
-        <f t="shared" si="3"/>
-        <v>6.392073828452719E-4</v>
+        <f t="shared" si="5"/>
+        <v>6.2667390475026658E-4</v>
       </c>
       <c r="G9" s="50">
-        <f t="shared" ref="G9:I9" si="7">G15/G$3</f>
-        <v>6.6823122234412231E-4</v>
+        <f t="shared" ref="G9:I9" si="9">G15/G$3</f>
+        <v>6.5512864935698273E-4</v>
       </c>
       <c r="H9" s="50">
-        <f t="shared" si="7"/>
-        <v>7.9832631468602867E-4</v>
+        <f t="shared" si="9"/>
+        <v>7.8267285753532215E-4</v>
       </c>
       <c r="I9" s="50">
-        <f t="shared" si="7"/>
-        <v>8.5193505352508189E-4</v>
+        <f t="shared" si="9"/>
+        <v>8.3523044463243326E-4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
@@ -3326,7 +3347,7 @@
         <v>103</v>
       </c>
       <c r="B11" s="38">
-        <f t="shared" ref="B11:B14" si="8">AVERAGE(E11:I11)</f>
+        <f t="shared" ref="B11:B14" si="10">AVERAGE(E11:I11)</f>
         <v>24502.799999999999</v>
       </c>
       <c r="C11" t="s">
@@ -3363,7 +3384,7 @@
         <v>104</v>
       </c>
       <c r="B12" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>26853</v>
       </c>
       <c r="D12" t="s">
@@ -3399,7 +3420,7 @@
         <v>105</v>
       </c>
       <c r="B13" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1215.2</v>
       </c>
       <c r="C13" s="15"/>
@@ -3436,7 +3457,7 @@
         <v>106</v>
       </c>
       <c r="B14" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1525.8</v>
       </c>
       <c r="C14" s="15"/>
@@ -3473,7 +3494,7 @@
         <v>107</v>
       </c>
       <c r="B15" s="38">
-        <f t="shared" ref="B15:B20" si="9">AVERAGE(E15:I15)</f>
+        <f t="shared" ref="B15:B20" si="11">AVERAGE(E15:I15)</f>
         <v>2152.4</v>
       </c>
       <c r="C15" s="15"/>
@@ -3510,7 +3531,7 @@
         <v>108</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>91046</v>
       </c>
       <c r="C16" s="2">
@@ -3542,7 +3563,7 @@
         <v>109</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>32124</v>
       </c>
       <c r="C17" s="2">
@@ -3574,7 +3595,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>412060000</v>
       </c>
       <c r="C18" s="4">
@@ -3613,7 +3634,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>90180000</v>
       </c>
       <c r="C19" s="4">
@@ -3652,35 +3673,35 @@
         <v>9</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>502240000</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" ref="C20:I20" si="10">SUM(C18:C19)</f>
+        <f t="shared" ref="C20:I20" si="12">SUM(C18:C19)</f>
         <v>506700000</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513100000</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>506600000</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>505400000</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>502900000</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>501900000</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>494400000</v>
       </c>
       <c r="J20" t="s">
@@ -3822,9 +3843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3862,23 +3883,28 @@
         <v>89</v>
       </c>
       <c r="B2" s="5">
-        <f t="shared" ref="B2:B15" si="0">AVERAGE(C2:E2)</f>
-        <v>363659</v>
+        <f>AVERAGE(C2:E2)*1.02</f>
+        <v>378350.8236</v>
       </c>
       <c r="C2" s="2">
-        <v>363659</v>
+        <f>363659*1.02</f>
+        <v>370932.18</v>
       </c>
       <c r="D2" s="2">
-        <v>363659</v>
+        <f t="shared" ref="D2:G3" si="0">363659*1.02</f>
+        <v>370932.18</v>
       </c>
       <c r="E2" s="2">
-        <v>363659</v>
+        <f t="shared" si="0"/>
+        <v>370932.18</v>
       </c>
       <c r="F2" s="2">
-        <v>363659</v>
+        <f t="shared" si="0"/>
+        <v>370932.18</v>
       </c>
       <c r="G2" s="2">
-        <v>363659</v>
+        <f t="shared" si="0"/>
+        <v>370932.18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -3886,23 +3912,28 @@
         <v>90</v>
       </c>
       <c r="B3" s="5">
+        <f>AVERAGE(C3:E3)*1.02</f>
+        <v>378350.8236</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:G3" si="1">363659*1.02</f>
+        <v>370932.18</v>
+      </c>
+      <c r="D3" s="2">
         <f t="shared" si="0"/>
-        <v>363659</v>
-      </c>
-      <c r="C3" s="2">
-        <v>363659</v>
-      </c>
-      <c r="D3" s="2">
-        <v>363659</v>
+        <v>370932.18</v>
       </c>
       <c r="E3" s="2">
-        <v>363659</v>
+        <f t="shared" si="0"/>
+        <v>370932.18</v>
       </c>
       <c r="F3" s="2">
-        <v>363659</v>
+        <f t="shared" si="0"/>
+        <v>370932.18</v>
       </c>
       <c r="G3" s="2">
-        <v>363659</v>
+        <f t="shared" si="0"/>
+        <v>370932.18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -3911,27 +3942,27 @@
       </c>
       <c r="B4" s="51">
         <f>AVERAGE(C4:E4)</f>
-        <v>8.2562922958045862E-2</v>
+        <v>8.0944042115731238E-2</v>
       </c>
       <c r="C4" s="50">
         <f>C10/C$2</f>
-        <v>8.1834905777115372E-2</v>
+        <v>8.0230299781485659E-2</v>
       </c>
       <c r="D4" s="50">
         <f>D10/D$2</f>
-        <v>8.0341748726141804E-2</v>
+        <v>7.8766420319746858E-2</v>
       </c>
       <c r="E4" s="50">
-        <f t="shared" ref="E4:G4" si="1">E10/E$2</f>
-        <v>8.551211437088041E-2</v>
+        <f t="shared" ref="E4:G4" si="2">E10/E$2</f>
+        <v>8.3835406245961197E-2</v>
       </c>
       <c r="F4" s="50">
-        <f t="shared" si="1"/>
-        <v>6.8606854223324604E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.7261621787573139E-2</v>
       </c>
       <c r="G4" s="50">
-        <f t="shared" si="1"/>
-        <v>7.3263689335338875E-2</v>
+        <f t="shared" si="2"/>
+        <v>7.1827146407194981E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -3940,27 +3971,27 @@
       </c>
       <c r="B5" s="51">
         <f>AVERAGE(C5:E5)</f>
-        <v>2.7520974319348621E-2</v>
+        <v>2.6981347371910411E-2</v>
       </c>
       <c r="C5" s="50">
         <f>C11/C$2</f>
-        <v>2.7278301925705125E-2</v>
+        <v>2.674343326049522E-2</v>
       </c>
       <c r="D5" s="50">
         <f>D11/D$2</f>
-        <v>2.6780582908713931E-2</v>
+        <v>2.6255473439915619E-2</v>
       </c>
       <c r="E5" s="50">
         <f>E11/E$2</f>
-        <v>2.8504038123626806E-2</v>
+        <v>2.7945135415320396E-2</v>
       </c>
       <c r="F5" s="50">
-        <f t="shared" ref="F5:G5" si="2">F11/F$2</f>
-        <v>2.2868951407774864E-2</v>
+        <f t="shared" ref="F5:G5" si="3">F11/F$2</f>
+        <v>2.2420540595857713E-2</v>
       </c>
       <c r="G5" s="50">
-        <f t="shared" si="2"/>
-        <v>2.4421229778446293E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.394238213573166E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -3969,27 +4000,27 @@
       </c>
       <c r="B6" s="51">
         <f>AVERAGE(C6:E6)</f>
-        <v>1.0388853293882457E-2</v>
+        <v>1.0185150288120054E-2</v>
       </c>
       <c r="C6" s="50">
-        <f t="shared" ref="C6:D9" si="3">C12/C$3</f>
-        <v>7.828762659524445E-3</v>
+        <f t="shared" ref="C6:D9" si="4">C12/C$3</f>
+        <v>7.6752575093376905E-3</v>
       </c>
       <c r="D6" s="50">
-        <f t="shared" si="3"/>
-        <v>1.045759901446135E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.0252548053393481E-2</v>
       </c>
       <c r="E6" s="50">
-        <f t="shared" ref="E6:G6" si="4">E12/E$3</f>
-        <v>1.2880198207661573E-2</v>
+        <f t="shared" ref="E6:G6" si="5">E12/E$3</f>
+        <v>1.2627645301628994E-2</v>
       </c>
       <c r="F6" s="50">
-        <f t="shared" si="4"/>
-        <v>1.3661149593437808E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.3393283915135107E-2</v>
       </c>
       <c r="G6" s="50">
-        <f t="shared" si="4"/>
-        <v>1.4821577356809539E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.4530958192950529E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -3998,27 +4029,27 @@
       </c>
       <c r="B7" s="51">
         <f>AVERAGE(C7:E7)</f>
-        <v>5.6279829913921198E-4</v>
+        <v>5.5176303837177639E-4</v>
       </c>
       <c r="C7" s="50">
-        <f t="shared" si="3"/>
-        <v>6.2421114285635723E-4</v>
+        <f t="shared" si="4"/>
+        <v>6.1197170868270312E-4</v>
       </c>
       <c r="D7" s="50">
-        <f t="shared" si="3"/>
-        <v>5.4996576463115171E-4</v>
+        <f t="shared" si="4"/>
+        <v>5.3918212218740367E-4</v>
       </c>
       <c r="E7" s="50">
-        <f t="shared" ref="E7:G7" si="5">E13/E$3</f>
-        <v>5.1421798993012688E-4</v>
+        <f t="shared" ref="E7:G7" si="6">E13/E$3</f>
+        <v>5.0413528424522237E-4</v>
       </c>
       <c r="F7" s="50">
-        <f t="shared" si="5"/>
-        <v>5.2521730522274988E-4</v>
+        <f t="shared" si="6"/>
+        <v>5.1491892668897052E-4</v>
       </c>
       <c r="G7" s="50">
-        <f t="shared" si="5"/>
-        <v>5.1696781875328263E-4</v>
+        <f t="shared" si="6"/>
+        <v>5.0683119485615943E-4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -4026,28 +4057,28 @@
         <v>29</v>
       </c>
       <c r="B8" s="51">
-        <f t="shared" si="0"/>
-        <v>1.5554865042984407E-3</v>
+        <f t="shared" ref="B2:B15" si="7">AVERAGE(C8:E8)</f>
+        <v>1.5249867689200401E-3</v>
       </c>
       <c r="C8" s="50">
-        <f t="shared" si="3"/>
-        <v>1.3034188621758296E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.2778616295841467E-3</v>
       </c>
       <c r="D8" s="50">
-        <f t="shared" si="3"/>
-        <v>1.6113996903692745E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.5798036180090928E-3</v>
       </c>
       <c r="E8" s="50">
-        <f t="shared" ref="E8:G8" si="6">E14/E$3</f>
-        <v>1.7516409603502182E-3</v>
+        <f t="shared" ref="E8:G8" si="8">E14/E$3</f>
+        <v>1.7172950591668806E-3</v>
       </c>
       <c r="F8" s="50">
-        <f t="shared" si="6"/>
-        <v>1.9551282932637444E-3</v>
+        <f t="shared" si="8"/>
+        <v>1.9167924443762199E-3</v>
       </c>
       <c r="G8" s="50">
-        <f t="shared" si="6"/>
-        <v>2.0816204191289093E-3</v>
+        <f t="shared" si="8"/>
+        <v>2.0408043324793229E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -4055,28 +4086,28 @@
         <v>31</v>
       </c>
       <c r="B9" s="51">
-        <f t="shared" si="0"/>
-        <v>9.413580671269881E-4</v>
+        <f t="shared" si="7"/>
+        <v>9.2290006581077257E-4</v>
       </c>
       <c r="C9" s="50">
-        <f t="shared" si="3"/>
-        <v>8.606964216477524E-4</v>
+        <f t="shared" si="4"/>
+        <v>8.438200212232867E-4</v>
       </c>
       <c r="D9" s="50">
-        <f t="shared" si="3"/>
-        <v>9.5419060163504826E-4</v>
+        <f t="shared" si="4"/>
+        <v>9.3548098199514528E-4</v>
       </c>
       <c r="E9" s="50">
-        <f t="shared" ref="E9:G9" si="7">E15/E$3</f>
-        <v>1.0091871780981633E-3</v>
+        <f t="shared" ref="E9:G9" si="9">E15/E$3</f>
+        <v>9.8939919421388561E-4</v>
       </c>
       <c r="F9" s="50">
-        <f t="shared" si="7"/>
-        <v>9.5144077281189251E-4</v>
+        <f t="shared" si="9"/>
+        <v>9.3278507138420833E-4</v>
       </c>
       <c r="G9" s="50">
-        <f t="shared" si="7"/>
-        <v>1.1081810157317707E-3</v>
+        <f t="shared" si="9"/>
+        <v>1.0864519762076184E-3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -4084,7 +4115,7 @@
         <v>98</v>
       </c>
       <c r="B10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>30024.75</v>
       </c>
       <c r="C10" s="2">
@@ -4166,7 +4197,7 @@
         <v>97</v>
       </c>
       <c r="B13" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>204.66666666666666</v>
       </c>
       <c r="C13" s="5">
@@ -4214,7 +4245,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>342.33333333333331</v>
       </c>
       <c r="C15" s="5">
@@ -4238,7 +4269,7 @@
         <v>94</v>
       </c>
       <c r="B16" s="5">
-        <f t="shared" ref="B16:B22" si="8">AVERAGE(C16:E16)</f>
+        <f t="shared" ref="B16:B22" si="10">AVERAGE(C16:E16)</f>
         <v>40033</v>
       </c>
       <c r="C16" s="5">
@@ -4262,7 +4293,7 @@
         <v>93</v>
       </c>
       <c r="B17" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4890.666666666667</v>
       </c>
       <c r="C17" s="5">
@@ -4341,7 +4372,7 @@
         <v>157913430</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" ref="D20" si="9">D22-D21</f>
+        <f t="shared" ref="D20" si="11">D22-D21</f>
         <v>154928604</v>
       </c>
       <c r="E20" s="3">
@@ -4362,7 +4393,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8927140.333333334</v>
       </c>
       <c r="C21" s="3">
@@ -4386,7 +4417,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>166732853</v>
       </c>
       <c r="C22" s="3">
@@ -4467,7 +4498,7 @@
         <v>56</v>
       </c>
       <c r="B29" s="35">
-        <f t="shared" ref="B29:B36" si="10">AVERAGE(C29:E29)</f>
+        <f t="shared" ref="B29:B36" si="12">AVERAGE(C29:E29)</f>
         <v>40033</v>
       </c>
       <c r="C29" s="2">
@@ -4485,7 +4516,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4897.666666666667</v>
       </c>
       <c r="C30" s="2">
@@ -4503,7 +4534,7 @@
         <v>58</v>
       </c>
       <c r="B31" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3778</v>
       </c>
       <c r="C31" s="2">
@@ -4521,7 +4552,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>204.66666666666666</v>
       </c>
       <c r="C32" s="2">
@@ -4539,7 +4570,7 @@
         <v>57</v>
       </c>
       <c r="B33" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>553.66666666666663</v>
       </c>
       <c r="C33" s="2">
@@ -4557,7 +4588,7 @@
         <v>60</v>
       </c>
       <c r="B34" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>331.66666666666669</v>
       </c>
       <c r="C34" s="2">
@@ -4575,7 +4606,7 @@
         <v>61</v>
       </c>
       <c r="B35" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>29.666666666666668</v>
       </c>
       <c r="C35" s="2">
@@ -4596,7 +4627,7 @@
         <v>62</v>
       </c>
       <c r="B36" s="35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>35135.333333333336</v>
       </c>
       <c r="C36" s="2">
@@ -4670,7 +4701,7 @@
         <v>67</v>
       </c>
       <c r="B41" s="35">
-        <f t="shared" ref="B41:B46" si="11">AVERAGE(C41:E41)</f>
+        <f t="shared" ref="B41:B46" si="13">AVERAGE(C41:E41)</f>
         <v>360781</v>
       </c>
       <c r="C41" s="2">
@@ -4688,7 +4719,7 @@
         <v>69</v>
       </c>
       <c r="B42" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>166732856.33333334</v>
       </c>
       <c r="C42" s="2">
@@ -4706,7 +4737,7 @@
         <v>66</v>
       </c>
       <c r="B43" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>509.10344432461801</v>
       </c>
       <c r="C43" s="2">
@@ -4727,7 +4758,7 @@
         <v>68</v>
       </c>
       <c r="B44" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>17381.333333333332</v>
       </c>
       <c r="C44" s="2">
@@ -4745,7 +4776,7 @@
         <v>70</v>
       </c>
       <c r="B45" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8927140.333333334</v>
       </c>
       <c r="C45" s="2">
@@ -4763,7 +4794,7 @@
         <v>71</v>
       </c>
       <c r="B46" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>175659996.66666666</v>
       </c>
       <c r="C46" s="2">
@@ -4797,11 +4828,11 @@
         <v>460.99570138551871</v>
       </c>
       <c r="D48" s="44">
-        <f t="shared" ref="D48:E48" si="12">D40/D$27*$G$27</f>
+        <f t="shared" ref="D48:E48" si="14">D40/D$27*$G$27</f>
         <v>443.97574119988997</v>
       </c>
       <c r="E48" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>433.36987122255812</v>
       </c>
     </row>
@@ -4810,7 +4841,7 @@
         <v>67</v>
       </c>
       <c r="B49" s="35">
-        <f t="shared" ref="B49:B54" si="13">AVERAGE(C49:E49)</f>
+        <f t="shared" ref="B49:B54" si="15">AVERAGE(C49:E49)</f>
         <v>360781</v>
       </c>
       <c r="C49" s="2">
@@ -4828,19 +4859,19 @@
         <v>69</v>
       </c>
       <c r="B50" s="43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>160900690.36601257</v>
       </c>
       <c r="C50" s="44">
-        <f t="shared" ref="C50:E51" si="14">C42/C$27*$G$27</f>
+        <f t="shared" ref="C50:E51" si="16">C42/C$27*$G$27</f>
         <v>164332520.66</v>
       </c>
       <c r="D50" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>159046317.72151896</v>
       </c>
       <c r="E50" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>159323232.71651879</v>
       </c>
     </row>
@@ -4849,19 +4880,19 @@
         <v>66</v>
       </c>
       <c r="B51" s="43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>491.24596549662516</v>
       </c>
       <c r="C51" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>510.8295355230332</v>
       </c>
       <c r="D51" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>503.18294805766584</v>
       </c>
       <c r="E51" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>459.72541290917655</v>
       </c>
     </row>
@@ -4870,7 +4901,7 @@
         <v>68</v>
       </c>
       <c r="B52" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>17381.333333333332</v>
       </c>
       <c r="C52" s="2">
@@ -4888,19 +4919,19 @@
         <v>70</v>
       </c>
       <c r="B53" s="43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>8605782.2879482117</v>
       </c>
       <c r="C53" s="44">
-        <f t="shared" ref="C53:E54" si="15">C45/C$27*$G$27</f>
+        <f t="shared" ref="C53:E54" si="17">C45/C$27*$G$27</f>
         <v>10715671.166666666</v>
       </c>
       <c r="D53" s="44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>8955146.9265822787</v>
       </c>
       <c r="E53" s="44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6146528.7705956912</v>
       </c>
     </row>
@@ -4909,19 +4940,19 @@
         <v>71</v>
       </c>
       <c r="B54" s="43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>169506472.65396079</v>
       </c>
       <c r="C54" s="44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>175048191.82666668</v>
       </c>
       <c r="D54" s="44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>168001464.64810127</v>
       </c>
       <c r="E54" s="44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>165469761.48711449</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ABF chunk temp fix, IB3 plot code, annual benefit cols v fixed. TBD - fix ABF chunk code
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AFA479-481D-4D4D-B3B9-3F8466BC4D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086897E1-9869-4C54-AA45-AFA168C07460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6930" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="338" yWindow="338" windowWidth="20677" windowHeight="12705" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_obsolote_Combined" sheetId="4" r:id="rId1"/>
@@ -2222,7 +2222,7 @@
         <v>13525678.380000001</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:I3" si="1">13260469*1.02</f>
+        <f t="shared" ref="E3" si="1">13260469*1.02</f>
         <v>13525678.380000001</v>
       </c>
       <c r="F3" s="2">
@@ -2276,7 +2276,7 @@
         <v>119</v>
       </c>
       <c r="B5" s="62">
-        <f t="shared" ref="B3:B20" si="4">AVERAGE(E5:I5)</f>
+        <f t="shared" ref="B5:B20" si="4">AVERAGE(E5:I5)</f>
         <v>1.2622124761774794E-2</v>
       </c>
       <c r="E5" s="54">
@@ -3114,7 +3114,7 @@
         <v>3046943.5308000003</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:I3" si="1">2928627*1.02</f>
+        <f t="shared" ref="E3" si="1">2928627*1.02</f>
         <v>2987199.54</v>
       </c>
       <c r="F3" s="2">
@@ -3845,7 +3845,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:G3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3860,7 +3860,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="52" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="52" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="C1" s="52">
         <v>2014</v>
@@ -3916,7 +3916,7 @@
         <v>378350.8236</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:G3" si="1">363659*1.02</f>
+        <f t="shared" ref="C3" si="1">363659*1.02</f>
         <v>370932.18</v>
       </c>
       <c r="D3" s="2">
@@ -4057,7 +4057,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="51">
-        <f t="shared" ref="B2:B15" si="7">AVERAGE(C8:E8)</f>
+        <f t="shared" ref="B8:B15" si="7">AVERAGE(C8:E8)</f>
         <v>1.5249867689200401E-3</v>
       </c>
       <c r="C8" s="50">

</xml_diff>

<commit_message>
FIXED cps-acs sim union/hourly, logit takeup bound issue. TBD abf chunk formal fix
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086897E1-9869-4C54-AA45-AFA168C07460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D4D7C6-6A7D-435F-9803-D20A3598A868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="338" yWindow="338" windowWidth="20677" windowHeight="12705" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23745" yWindow="8340" windowWidth="20430" windowHeight="12510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_obsolote_Combined" sheetId="4" r:id="rId1"/>
@@ -2141,11 +2141,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4:B9"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3023,10 +3023,10 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4:B9"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3079,8 +3079,8 @@
         <v>89</v>
       </c>
       <c r="B2" s="2">
-        <f>AVERAGE(E2:I2)*1.02</f>
-        <v>3046943.5308000003</v>
+        <f>AVERAGE(E2:I2)</f>
+        <v>2987199.54</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -3110,8 +3110,8 @@
         <v>90</v>
       </c>
       <c r="B3" s="2">
-        <f>AVERAGE(E3:I3)*1.02</f>
-        <v>3046943.5308000003</v>
+        <f>AVERAGE(E3:I3)</f>
+        <v>2987199.54</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3" si="1">2928627*1.02</f>
@@ -3843,9 +3843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3883,27 +3883,27 @@
         <v>89</v>
       </c>
       <c r="B2" s="5">
-        <f>AVERAGE(C2:E2)*1.02</f>
-        <v>378350.8236</v>
+        <f t="shared" ref="B2:B7" si="0">AVERAGE(C2:E2)</f>
+        <v>370932.18</v>
       </c>
       <c r="C2" s="2">
         <f>363659*1.02</f>
         <v>370932.18</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:G3" si="0">363659*1.02</f>
+        <f t="shared" ref="D2:G3" si="1">363659*1.02</f>
         <v>370932.18</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>370932.18</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>370932.18</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>370932.18</v>
       </c>
     </row>
@@ -3912,27 +3912,27 @@
         <v>90</v>
       </c>
       <c r="B3" s="5">
-        <f>AVERAGE(C3:E3)*1.02</f>
-        <v>378350.8236</v>
-      </c>
-      <c r="C3" s="2">
-        <f t="shared" ref="C3" si="1">363659*1.02</f>
-        <v>370932.18</v>
-      </c>
-      <c r="D3" s="2">
         <f t="shared" si="0"/>
         <v>370932.18</v>
       </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3" si="2">363659*1.02</f>
+        <v>370932.18</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" si="1"/>
+        <v>370932.18</v>
+      </c>
       <c r="E3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>370932.18</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>370932.18</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>370932.18</v>
       </c>
     </row>
@@ -3941,7 +3941,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="51">
-        <f>AVERAGE(C4:E4)</f>
+        <f t="shared" si="0"/>
         <v>8.0944042115731238E-2</v>
       </c>
       <c r="C4" s="50">
@@ -3953,15 +3953,15 @@
         <v>7.8766420319746858E-2</v>
       </c>
       <c r="E4" s="50">
-        <f t="shared" ref="E4:G4" si="2">E10/E$2</f>
+        <f t="shared" ref="E4:G4" si="3">E10/E$2</f>
         <v>8.3835406245961197E-2</v>
       </c>
       <c r="F4" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.7261621787573139E-2</v>
       </c>
       <c r="G4" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1827146407194981E-2</v>
       </c>
     </row>
@@ -3970,7 +3970,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="51">
-        <f>AVERAGE(C5:E5)</f>
+        <f t="shared" si="0"/>
         <v>2.6981347371910411E-2</v>
       </c>
       <c r="C5" s="50">
@@ -3986,11 +3986,11 @@
         <v>2.7945135415320396E-2</v>
       </c>
       <c r="F5" s="50">
-        <f t="shared" ref="F5:G5" si="3">F11/F$2</f>
+        <f t="shared" ref="F5:G5" si="4">F11/F$2</f>
         <v>2.2420540595857713E-2</v>
       </c>
       <c r="G5" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.394238213573166E-2</v>
       </c>
     </row>
@@ -3999,27 +3999,27 @@
         <v>33</v>
       </c>
       <c r="B6" s="51">
-        <f>AVERAGE(C6:E6)</f>
+        <f t="shared" si="0"/>
         <v>1.0185150288120054E-2</v>
       </c>
       <c r="C6" s="50">
-        <f t="shared" ref="C6:D9" si="4">C12/C$3</f>
+        <f t="shared" ref="C6:D9" si="5">C12/C$3</f>
         <v>7.6752575093376905E-3</v>
       </c>
       <c r="D6" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0252548053393481E-2</v>
       </c>
       <c r="E6" s="50">
-        <f t="shared" ref="E6:G6" si="5">E12/E$3</f>
+        <f t="shared" ref="E6:G6" si="6">E12/E$3</f>
         <v>1.2627645301628994E-2</v>
       </c>
       <c r="F6" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3393283915135107E-2</v>
       </c>
       <c r="G6" s="50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4530958192950529E-2</v>
       </c>
     </row>
@@ -4032,23 +4032,23 @@
         <v>5.5176303837177639E-4</v>
       </c>
       <c r="C7" s="50">
-        <f t="shared" si="4"/>
+        <f>C13/C$3</f>
         <v>6.1197170868270312E-4</v>
       </c>
       <c r="D7" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.3918212218740367E-4</v>
       </c>
       <c r="E7" s="50">
-        <f t="shared" ref="E7:G7" si="6">E13/E$3</f>
+        <f t="shared" ref="E7:G7" si="7">E13/E$3</f>
         <v>5.0413528424522237E-4</v>
       </c>
       <c r="F7" s="50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.1491892668897052E-4</v>
       </c>
       <c r="G7" s="50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.0683119485615943E-4</v>
       </c>
     </row>
@@ -4057,27 +4057,27 @@
         <v>29</v>
       </c>
       <c r="B8" s="51">
-        <f t="shared" ref="B8:B15" si="7">AVERAGE(C8:E8)</f>
+        <f t="shared" ref="B8:B15" si="8">AVERAGE(C8:E8)</f>
         <v>1.5249867689200401E-3</v>
       </c>
       <c r="C8" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2778616295841467E-3</v>
       </c>
       <c r="D8" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5798036180090928E-3</v>
       </c>
       <c r="E8" s="50">
-        <f t="shared" ref="E8:G8" si="8">E14/E$3</f>
+        <f t="shared" ref="E8:G8" si="9">E14/E$3</f>
         <v>1.7172950591668806E-3</v>
       </c>
       <c r="F8" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.9167924443762199E-3</v>
       </c>
       <c r="G8" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0408043324793229E-3</v>
       </c>
     </row>
@@ -4086,27 +4086,27 @@
         <v>31</v>
       </c>
       <c r="B9" s="51">
-        <f t="shared" si="7"/>
+        <f>AVERAGE(C9:E9)</f>
         <v>9.2290006581077257E-4</v>
       </c>
       <c r="C9" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.438200212232867E-4</v>
       </c>
       <c r="D9" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.3548098199514528E-4</v>
       </c>
       <c r="E9" s="50">
-        <f t="shared" ref="E9:G9" si="9">E15/E$3</f>
+        <f t="shared" ref="E9:G9" si="10">E15/E$3</f>
         <v>9.8939919421388561E-4</v>
       </c>
       <c r="F9" s="50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.3278507138420833E-4</v>
       </c>
       <c r="G9" s="50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.0864519762076184E-3</v>
       </c>
     </row>
@@ -4115,7 +4115,7 @@
         <v>98</v>
       </c>
       <c r="B10" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>30024.75</v>
       </c>
       <c r="C10" s="2">
@@ -4197,7 +4197,7 @@
         <v>97</v>
       </c>
       <c r="B13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>204.66666666666666</v>
       </c>
       <c r="C13" s="5">
@@ -4245,7 +4245,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>342.33333333333331</v>
       </c>
       <c r="C15" s="5">
@@ -4269,7 +4269,7 @@
         <v>94</v>
       </c>
       <c r="B16" s="5">
-        <f t="shared" ref="B16:B22" si="10">AVERAGE(C16:E16)</f>
+        <f t="shared" ref="B16:B22" si="11">AVERAGE(C16:E16)</f>
         <v>40033</v>
       </c>
       <c r="C16" s="5">
@@ -4293,7 +4293,7 @@
         <v>93</v>
       </c>
       <c r="B17" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4890.666666666667</v>
       </c>
       <c r="C17" s="5">
@@ -4372,7 +4372,7 @@
         <v>157913430</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" ref="D20" si="11">D22-D21</f>
+        <f t="shared" ref="D20" si="12">D22-D21</f>
         <v>154928604</v>
       </c>
       <c r="E20" s="3">
@@ -4393,7 +4393,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8927140.333333334</v>
       </c>
       <c r="C21" s="3">
@@ -4417,7 +4417,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>166732853</v>
       </c>
       <c r="C22" s="3">
@@ -4434,6 +4434,12 @@
       </c>
       <c r="G22" s="3">
         <v>187110769</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B23" s="9">
+        <f>SUM(B10:B15)</f>
+        <v>44923.666666666664</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
@@ -4498,7 +4504,7 @@
         <v>56</v>
       </c>
       <c r="B29" s="35">
-        <f t="shared" ref="B29:B36" si="12">AVERAGE(C29:E29)</f>
+        <f t="shared" ref="B29:B36" si="13">AVERAGE(C29:E29)</f>
         <v>40033</v>
       </c>
       <c r="C29" s="2">
@@ -4516,7 +4522,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4897.666666666667</v>
       </c>
       <c r="C30" s="2">
@@ -4534,7 +4540,7 @@
         <v>58</v>
       </c>
       <c r="B31" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3778</v>
       </c>
       <c r="C31" s="2">
@@ -4552,7 +4558,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>204.66666666666666</v>
       </c>
       <c r="C32" s="2">
@@ -4570,7 +4576,7 @@
         <v>57</v>
       </c>
       <c r="B33" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>553.66666666666663</v>
       </c>
       <c r="C33" s="2">
@@ -4588,7 +4594,7 @@
         <v>60</v>
       </c>
       <c r="B34" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>331.66666666666669</v>
       </c>
       <c r="C34" s="2">
@@ -4606,7 +4612,7 @@
         <v>61</v>
       </c>
       <c r="B35" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29.666666666666668</v>
       </c>
       <c r="C35" s="2">
@@ -4627,7 +4633,7 @@
         <v>62</v>
       </c>
       <c r="B36" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>35135.333333333336</v>
       </c>
       <c r="C36" s="2">
@@ -4701,7 +4707,7 @@
         <v>67</v>
       </c>
       <c r="B41" s="35">
-        <f t="shared" ref="B41:B46" si="13">AVERAGE(C41:E41)</f>
+        <f t="shared" ref="B41:B46" si="14">AVERAGE(C41:E41)</f>
         <v>360781</v>
       </c>
       <c r="C41" s="2">
@@ -4719,7 +4725,7 @@
         <v>69</v>
       </c>
       <c r="B42" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>166732856.33333334</v>
       </c>
       <c r="C42" s="2">
@@ -4737,7 +4743,7 @@
         <v>66</v>
       </c>
       <c r="B43" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>509.10344432461801</v>
       </c>
       <c r="C43" s="2">
@@ -4758,7 +4764,7 @@
         <v>68</v>
       </c>
       <c r="B44" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>17381.333333333332</v>
       </c>
       <c r="C44" s="2">
@@ -4776,7 +4782,7 @@
         <v>70</v>
       </c>
       <c r="B45" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8927140.333333334</v>
       </c>
       <c r="C45" s="2">
@@ -4794,7 +4800,7 @@
         <v>71</v>
       </c>
       <c r="B46" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>175659996.66666666</v>
       </c>
       <c r="C46" s="2">
@@ -4828,11 +4834,11 @@
         <v>460.99570138551871</v>
       </c>
       <c r="D48" s="44">
-        <f t="shared" ref="D48:E48" si="14">D40/D$27*$G$27</f>
+        <f t="shared" ref="D48:E48" si="15">D40/D$27*$G$27</f>
         <v>443.97574119988997</v>
       </c>
       <c r="E48" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>433.36987122255812</v>
       </c>
     </row>
@@ -4841,7 +4847,7 @@
         <v>67</v>
       </c>
       <c r="B49" s="35">
-        <f t="shared" ref="B49:B54" si="15">AVERAGE(C49:E49)</f>
+        <f t="shared" ref="B49:B54" si="16">AVERAGE(C49:E49)</f>
         <v>360781</v>
       </c>
       <c r="C49" s="2">
@@ -4859,19 +4865,19 @@
         <v>69</v>
       </c>
       <c r="B50" s="43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>160900690.36601257</v>
       </c>
       <c r="C50" s="44">
-        <f t="shared" ref="C50:E51" si="16">C42/C$27*$G$27</f>
+        <f t="shared" ref="C50:E51" si="17">C42/C$27*$G$27</f>
         <v>164332520.66</v>
       </c>
       <c r="D50" s="44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>159046317.72151896</v>
       </c>
       <c r="E50" s="44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>159323232.71651879</v>
       </c>
     </row>
@@ -4880,19 +4886,19 @@
         <v>66</v>
       </c>
       <c r="B51" s="43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>491.24596549662516</v>
       </c>
       <c r="C51" s="44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>510.8295355230332</v>
       </c>
       <c r="D51" s="44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>503.18294805766584</v>
       </c>
       <c r="E51" s="44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>459.72541290917655</v>
       </c>
     </row>
@@ -4901,7 +4907,7 @@
         <v>68</v>
       </c>
       <c r="B52" s="35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>17381.333333333332</v>
       </c>
       <c r="C52" s="2">
@@ -4919,19 +4925,19 @@
         <v>70</v>
       </c>
       <c r="B53" s="43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8605782.2879482117</v>
       </c>
       <c r="C53" s="44">
-        <f t="shared" ref="C53:E54" si="17">C45/C$27*$G$27</f>
+        <f t="shared" ref="C53:E54" si="18">C45/C$27*$G$27</f>
         <v>10715671.166666666</v>
       </c>
       <c r="D53" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8955146.9265822787</v>
       </c>
       <c r="E53" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6146528.7705956912</v>
       </c>
     </row>
@@ -4940,19 +4946,19 @@
         <v>71</v>
       </c>
       <c r="B54" s="43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>169506472.65396079</v>
       </c>
       <c r="C54" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>175048191.82666668</v>
       </c>
       <c r="D54" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>168001464.64810127</v>
       </c>
       <c r="E54" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>165469761.48711449</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed ABF population results by 1.02X for POW=True
</commit_message>
<xml_diff>
--- a/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
+++ b/state_program_statistics/Actual Leave Data 2014-2018_CZ.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workfiles\Microsimulation\microsim\state_program_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D4D7C6-6A7D-435F-9803-D20A3598A868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C82302-D8C6-45F7-AFD4-D6641F60898C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23745" yWindow="8340" windowWidth="20430" windowHeight="12510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24945" yWindow="10815" windowWidth="12840" windowHeight="7800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_obsolote_Combined" sheetId="4" r:id="rId1"/>
     <sheet name="California" sheetId="1" r:id="rId2"/>
     <sheet name="New Jersey" sheetId="2" r:id="rId3"/>
     <sheet name="Rhode Island" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="ca_PLF_breakdown" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -504,6 +504,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2141,11 +2142,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2521,7 +2522,7 @@
         <v>124</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(E13:I13)</f>
         <v>6400.7132799999999</v>
       </c>
       <c r="C13" s="25">
@@ -3022,11 +3023,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:B11"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3845,7 +3846,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10:B15"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3883,7 +3884,7 @@
         <v>89</v>
       </c>
       <c r="B2" s="5">
-        <f t="shared" ref="B2:B7" si="0">AVERAGE(C2:E2)</f>
+        <f t="shared" ref="B2:B6" si="0">AVERAGE(C2:E2)</f>
         <v>370932.18</v>
       </c>
       <c r="C2" s="2">
@@ -5005,7 +5006,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:J14"/>
+      <selection activeCell="B13" sqref="A1:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>